<commit_message>
feat: add projeto backend da local farm em java
</commit_message>
<xml_diff>
--- a/Sprints/Sprint 8 - dia 20_05_2024 (será entregue)/Planilha de Testes/Planilha de Teste.xlsx
+++ b/Sprints/Sprint 8 - dia 20_05_2024 (será entregue)/Planilha de Testes/Planilha de Teste.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\Documents\Teste-Planilha\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\Documents\backlogs\Sprints\Sprint 8 - dia 20_05_2024 (será entregue)\Planilha de Testes\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -497,26 +497,14 @@
     <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -527,6 +515,18 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -536,14 +536,14 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -827,31 +827,31 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:H152"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A154" workbookViewId="0">
-      <selection activeCell="H148" sqref="H148"/>
+    <sheetView tabSelected="1" zoomScale="40" zoomScaleNormal="40" workbookViewId="0">
+      <selection activeCell="G2" sqref="G2:H5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="2" max="2" width="29.7109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="28.140625" customWidth="1"/>
-    <col min="4" max="4" width="37.140625" customWidth="1"/>
-    <col min="7" max="7" width="12.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="29.7265625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="28.1796875" customWidth="1"/>
+    <col min="4" max="4" width="37.1796875" customWidth="1"/>
+    <col min="7" max="7" width="12.1796875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:8" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="B2" s="4" t="s">
+    <row r="2" spans="2:8" ht="18.5" x14ac:dyDescent="0.45">
+      <c r="B2" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="4"/>
-      <c r="D2" s="4"/>
-      <c r="E2" s="4"/>
+      <c r="C2" s="2"/>
+      <c r="D2" s="2"/>
+      <c r="E2" s="2"/>
       <c r="G2" s="12" t="s">
         <v>4</v>
       </c>
       <c r="H2" s="12"/>
     </row>
-    <row r="3" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:8" x14ac:dyDescent="0.35">
       <c r="B3" s="1" t="s">
         <v>1</v>
       </c>
@@ -869,269 +869,269 @@
       </c>
       <c r="H3" s="14"/>
     </row>
-    <row r="4" spans="2:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B4" s="5" t="s">
+    <row r="4" spans="2:8" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B4" s="11" t="s">
         <v>5</v>
       </c>
       <c r="C4" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="D4" s="6" t="s">
+      <c r="D4" s="15" t="s">
         <v>33</v>
       </c>
-      <c r="E4" s="9"/>
+      <c r="E4" s="5"/>
       <c r="G4" s="13" t="s">
         <v>20</v>
       </c>
       <c r="H4" s="14"/>
     </row>
-    <row r="5" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B5" s="5"/>
+    <row r="5" spans="2:8" x14ac:dyDescent="0.35">
+      <c r="B5" s="11"/>
       <c r="C5" s="3"/>
-      <c r="D5" s="7"/>
-      <c r="E5" s="10"/>
+      <c r="D5" s="16"/>
+      <c r="E5" s="6"/>
       <c r="G5" s="13" t="s">
         <v>21</v>
       </c>
       <c r="H5" s="14"/>
     </row>
-    <row r="6" spans="2:8" ht="57" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B6" s="5"/>
+    <row r="6" spans="2:8" ht="57" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B6" s="11"/>
       <c r="C6" s="3"/>
-      <c r="D6" s="8"/>
-      <c r="E6" s="10"/>
-    </row>
-    <row r="7" spans="2:8" ht="75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B7" s="5"/>
+      <c r="D6" s="17"/>
+      <c r="E6" s="6"/>
+    </row>
+    <row r="7" spans="2:8" ht="75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B7" s="11"/>
       <c r="C7" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="D7" s="6" t="s">
+      <c r="D7" s="15" t="s">
         <v>34</v>
       </c>
-      <c r="E7" s="10"/>
-    </row>
-    <row r="8" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B8" s="5"/>
+      <c r="E7" s="6"/>
+    </row>
+    <row r="8" spans="2:8" x14ac:dyDescent="0.35">
+      <c r="B8" s="11"/>
       <c r="C8" s="3"/>
-      <c r="D8" s="7"/>
-      <c r="E8" s="10"/>
-    </row>
-    <row r="9" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B9" s="5"/>
+      <c r="D8" s="16"/>
+      <c r="E8" s="6"/>
+    </row>
+    <row r="9" spans="2:8" x14ac:dyDescent="0.35">
+      <c r="B9" s="11"/>
       <c r="C9" s="3"/>
-      <c r="D9" s="8"/>
-      <c r="E9" s="11"/>
-    </row>
-    <row r="10" spans="2:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B10" s="2" t="s">
+      <c r="D9" s="17"/>
+      <c r="E9" s="7"/>
+    </row>
+    <row r="10" spans="2:8" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B10" s="4" t="s">
         <v>7</v>
       </c>
       <c r="C10" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="D10" s="6" t="s">
+      <c r="D10" s="15" t="s">
         <v>35</v>
       </c>
-      <c r="E10" s="9"/>
-    </row>
-    <row r="11" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B11" s="2"/>
+      <c r="E10" s="5"/>
+    </row>
+    <row r="11" spans="2:8" x14ac:dyDescent="0.35">
+      <c r="B11" s="4"/>
       <c r="C11" s="3"/>
-      <c r="D11" s="7"/>
-      <c r="E11" s="10"/>
-    </row>
-    <row r="12" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B12" s="2"/>
+      <c r="D11" s="16"/>
+      <c r="E11" s="6"/>
+    </row>
+    <row r="12" spans="2:8" x14ac:dyDescent="0.35">
+      <c r="B12" s="4"/>
       <c r="C12" s="3"/>
-      <c r="D12" s="8"/>
-      <c r="E12" s="10"/>
-    </row>
-    <row r="13" spans="2:8" ht="105" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B13" s="2"/>
+      <c r="D12" s="17"/>
+      <c r="E12" s="6"/>
+    </row>
+    <row r="13" spans="2:8" ht="105" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B13" s="4"/>
       <c r="C13" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="D13" s="6" t="s">
+      <c r="D13" s="15" t="s">
         <v>36</v>
       </c>
-      <c r="E13" s="10"/>
-    </row>
-    <row r="14" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B14" s="2"/>
+      <c r="E13" s="6"/>
+    </row>
+    <row r="14" spans="2:8" x14ac:dyDescent="0.35">
+      <c r="B14" s="4"/>
       <c r="C14" s="3"/>
-      <c r="D14" s="7"/>
-      <c r="E14" s="10"/>
-    </row>
-    <row r="15" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B15" s="2"/>
+      <c r="D14" s="16"/>
+      <c r="E14" s="6"/>
+    </row>
+    <row r="15" spans="2:8" x14ac:dyDescent="0.35">
+      <c r="B15" s="4"/>
       <c r="C15" s="3"/>
-      <c r="D15" s="8"/>
-      <c r="E15" s="10"/>
-    </row>
-    <row r="16" spans="2:8" ht="105" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B16" s="2"/>
+      <c r="D15" s="17"/>
+      <c r="E15" s="6"/>
+    </row>
+    <row r="16" spans="2:8" ht="105" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B16" s="4"/>
       <c r="C16" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="D16" s="6" t="s">
+      <c r="D16" s="15" t="s">
         <v>37</v>
       </c>
-      <c r="E16" s="10"/>
-    </row>
-    <row r="17" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B17" s="2"/>
+      <c r="E16" s="6"/>
+    </row>
+    <row r="17" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="B17" s="4"/>
       <c r="C17" s="3"/>
-      <c r="D17" s="7"/>
-      <c r="E17" s="10"/>
-    </row>
-    <row r="18" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B18" s="2"/>
+      <c r="D17" s="16"/>
+      <c r="E17" s="6"/>
+    </row>
+    <row r="18" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="B18" s="4"/>
       <c r="C18" s="3"/>
-      <c r="D18" s="8"/>
-      <c r="E18" s="11"/>
-    </row>
-    <row r="19" spans="2:5" ht="75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B19" s="2" t="s">
+      <c r="D18" s="17"/>
+      <c r="E18" s="7"/>
+    </row>
+    <row r="19" spans="2:5" ht="75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B19" s="4" t="s">
         <v>11</v>
       </c>
       <c r="C19" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="D19" s="6" t="s">
+      <c r="D19" s="15" t="s">
         <v>38</v>
       </c>
-      <c r="E19" s="9"/>
-    </row>
-    <row r="20" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B20" s="2"/>
+      <c r="E19" s="5"/>
+    </row>
+    <row r="20" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="B20" s="4"/>
       <c r="C20" s="3"/>
-      <c r="D20" s="7"/>
-      <c r="E20" s="10"/>
-    </row>
-    <row r="21" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B21" s="2"/>
+      <c r="D20" s="16"/>
+      <c r="E20" s="6"/>
+    </row>
+    <row r="21" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="B21" s="4"/>
       <c r="C21" s="3"/>
-      <c r="D21" s="7"/>
-      <c r="E21" s="10"/>
-    </row>
-    <row r="22" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B22" s="2"/>
+      <c r="D21" s="16"/>
+      <c r="E21" s="6"/>
+    </row>
+    <row r="22" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="B22" s="4"/>
       <c r="C22" s="3"/>
-      <c r="D22" s="8"/>
-      <c r="E22" s="10"/>
-    </row>
-    <row r="23" spans="2:5" ht="60" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B23" s="2"/>
+      <c r="D22" s="17"/>
+      <c r="E22" s="6"/>
+    </row>
+    <row r="23" spans="2:5" ht="60" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B23" s="4"/>
       <c r="C23" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="D23" s="6" t="s">
+      <c r="D23" s="15" t="s">
         <v>39</v>
       </c>
-      <c r="E23" s="10"/>
-    </row>
-    <row r="24" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B24" s="2"/>
+      <c r="E23" s="6"/>
+    </row>
+    <row r="24" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="B24" s="4"/>
       <c r="C24" s="3"/>
-      <c r="D24" s="7"/>
-      <c r="E24" s="10"/>
-    </row>
-    <row r="25" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B25" s="2"/>
+      <c r="D24" s="16"/>
+      <c r="E24" s="6"/>
+    </row>
+    <row r="25" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="B25" s="4"/>
       <c r="C25" s="3"/>
-      <c r="D25" s="8"/>
-      <c r="E25" s="11"/>
-    </row>
-    <row r="26" spans="2:5" ht="105" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B26" s="2" t="s">
+      <c r="D25" s="17"/>
+      <c r="E25" s="7"/>
+    </row>
+    <row r="26" spans="2:5" ht="105" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B26" s="4" t="s">
         <v>15</v>
       </c>
       <c r="C26" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="D26" s="6" t="s">
+      <c r="D26" s="15" t="s">
         <v>40</v>
       </c>
-      <c r="E26" s="9"/>
-    </row>
-    <row r="27" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B27" s="2"/>
+      <c r="E26" s="5"/>
+    </row>
+    <row r="27" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="B27" s="4"/>
       <c r="C27" s="3"/>
-      <c r="D27" s="7"/>
-      <c r="E27" s="10"/>
-    </row>
-    <row r="28" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B28" s="2"/>
+      <c r="D27" s="16"/>
+      <c r="E27" s="6"/>
+    </row>
+    <row r="28" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="B28" s="4"/>
       <c r="C28" s="3"/>
-      <c r="D28" s="7"/>
-      <c r="E28" s="10"/>
-    </row>
-    <row r="29" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B29" s="2"/>
+      <c r="D28" s="16"/>
+      <c r="E28" s="6"/>
+    </row>
+    <row r="29" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="B29" s="4"/>
       <c r="C29" s="3"/>
-      <c r="D29" s="8"/>
-      <c r="E29" s="10"/>
-    </row>
-    <row r="30" spans="2:5" ht="75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B30" s="2"/>
+      <c r="D29" s="17"/>
+      <c r="E29" s="6"/>
+    </row>
+    <row r="30" spans="2:5" ht="75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B30" s="4"/>
       <c r="C30" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="D30" s="6" t="s">
+      <c r="D30" s="15" t="s">
         <v>41</v>
       </c>
-      <c r="E30" s="10"/>
-    </row>
-    <row r="31" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B31" s="2"/>
+      <c r="E30" s="6"/>
+    </row>
+    <row r="31" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="B31" s="4"/>
       <c r="C31" s="3"/>
-      <c r="D31" s="7"/>
-      <c r="E31" s="10"/>
-    </row>
-    <row r="32" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B32" s="2"/>
+      <c r="D31" s="16"/>
+      <c r="E31" s="6"/>
+    </row>
+    <row r="32" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="B32" s="4"/>
       <c r="C32" s="3"/>
-      <c r="D32" s="7"/>
-      <c r="E32" s="10"/>
-    </row>
-    <row r="33" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B33" s="2"/>
+      <c r="D32" s="16"/>
+      <c r="E32" s="6"/>
+    </row>
+    <row r="33" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="B33" s="4"/>
       <c r="C33" s="3"/>
-      <c r="D33" s="8"/>
-      <c r="E33" s="10"/>
-    </row>
-    <row r="34" spans="2:5" ht="90" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B34" s="2"/>
+      <c r="D33" s="17"/>
+      <c r="E33" s="6"/>
+    </row>
+    <row r="34" spans="2:5" ht="90" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B34" s="4"/>
       <c r="C34" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="D34" s="6" t="s">
+      <c r="D34" s="15" t="s">
         <v>42</v>
       </c>
-      <c r="E34" s="10"/>
-    </row>
-    <row r="35" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B35" s="2"/>
+      <c r="E34" s="6"/>
+    </row>
+    <row r="35" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="B35" s="4"/>
       <c r="C35" s="3"/>
-      <c r="D35" s="7"/>
-      <c r="E35" s="10"/>
-    </row>
-    <row r="36" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B36" s="2"/>
+      <c r="D35" s="16"/>
+      <c r="E35" s="6"/>
+    </row>
+    <row r="36" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="B36" s="4"/>
       <c r="C36" s="3"/>
-      <c r="D36" s="8"/>
-      <c r="E36" s="11"/>
-    </row>
-    <row r="39" spans="2:5" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="B39" s="4" t="s">
+      <c r="D36" s="17"/>
+      <c r="E36" s="7"/>
+    </row>
+    <row r="39" spans="2:5" ht="18.5" x14ac:dyDescent="0.45">
+      <c r="B39" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="C39" s="4"/>
-      <c r="D39" s="4"/>
-      <c r="E39" s="4"/>
-    </row>
-    <row r="40" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="C39" s="2"/>
+      <c r="D39" s="2"/>
+      <c r="E39" s="2"/>
+    </row>
+    <row r="40" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B40" s="1" t="s">
         <v>1</v>
       </c>
@@ -1145,8 +1145,8 @@
         <v>4</v>
       </c>
     </row>
-    <row r="41" spans="2:5" ht="75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B41" s="2" t="s">
+    <row r="41" spans="2:5" ht="75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B41" s="4" t="s">
         <v>23</v>
       </c>
       <c r="C41" s="3" t="s">
@@ -1155,66 +1155,66 @@
       <c r="D41" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="E41" s="15"/>
-    </row>
-    <row r="42" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B42" s="2"/>
+      <c r="E41" s="9"/>
+    </row>
+    <row r="42" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="B42" s="4"/>
       <c r="C42" s="3"/>
       <c r="D42" s="3"/>
-      <c r="E42" s="15"/>
-    </row>
-    <row r="43" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B43" s="2"/>
+      <c r="E42" s="9"/>
+    </row>
+    <row r="43" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="B43" s="4"/>
       <c r="C43" s="3"/>
       <c r="D43" s="3"/>
-      <c r="E43" s="15"/>
-    </row>
-    <row r="44" spans="2:5" ht="75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B44" s="2"/>
+      <c r="E43" s="9"/>
+    </row>
+    <row r="44" spans="2:5" ht="75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B44" s="4"/>
       <c r="C44" s="3" t="s">
         <v>25</v>
       </c>
       <c r="D44" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="E44" s="15"/>
-    </row>
-    <row r="45" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B45" s="2"/>
+      <c r="E44" s="9"/>
+    </row>
+    <row r="45" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="B45" s="4"/>
       <c r="C45" s="3"/>
       <c r="D45" s="3"/>
-      <c r="E45" s="15"/>
-    </row>
-    <row r="46" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B46" s="2"/>
+      <c r="E45" s="9"/>
+    </row>
+    <row r="46" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="B46" s="4"/>
       <c r="C46" s="3"/>
       <c r="D46" s="3"/>
-      <c r="E46" s="15"/>
-    </row>
-    <row r="47" spans="2:5" ht="60" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B47" s="2"/>
+      <c r="E46" s="9"/>
+    </row>
+    <row r="47" spans="2:5" ht="60" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B47" s="4"/>
       <c r="C47" s="3" t="s">
         <v>26</v>
       </c>
       <c r="D47" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="E47" s="15"/>
-    </row>
-    <row r="48" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B48" s="2"/>
+      <c r="E47" s="9"/>
+    </row>
+    <row r="48" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="B48" s="4"/>
       <c r="C48" s="3"/>
       <c r="D48" s="3"/>
-      <c r="E48" s="15"/>
-    </row>
-    <row r="49" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B49" s="2"/>
+      <c r="E48" s="9"/>
+    </row>
+    <row r="49" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="B49" s="4"/>
       <c r="C49" s="3"/>
       <c r="D49" s="3"/>
-      <c r="E49" s="15"/>
-    </row>
-    <row r="50" spans="2:5" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B50" s="2" t="s">
+      <c r="E49" s="9"/>
+    </row>
+    <row r="50" spans="2:5" ht="45" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B50" s="4" t="s">
         <v>30</v>
       </c>
       <c r="C50" s="3" t="s">
@@ -1223,29 +1223,29 @@
       <c r="D50" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="E50" s="9"/>
-    </row>
-    <row r="51" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B51" s="2"/>
+      <c r="E50" s="5"/>
+    </row>
+    <row r="51" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="B51" s="4"/>
       <c r="C51" s="3"/>
       <c r="D51" s="3"/>
-      <c r="E51" s="10"/>
-    </row>
-    <row r="52" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B52" s="2"/>
+      <c r="E51" s="6"/>
+    </row>
+    <row r="52" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="B52" s="4"/>
       <c r="C52" s="3"/>
       <c r="D52" s="3"/>
-      <c r="E52" s="11"/>
-    </row>
-    <row r="55" spans="2:5" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="B55" s="4" t="s">
+      <c r="E52" s="7"/>
+    </row>
+    <row r="55" spans="2:5" ht="18.5" x14ac:dyDescent="0.45">
+      <c r="B55" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="C55" s="4"/>
-      <c r="D55" s="4"/>
-      <c r="E55" s="4"/>
-    </row>
-    <row r="56" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="C55" s="2"/>
+      <c r="D55" s="2"/>
+      <c r="E55" s="2"/>
+    </row>
+    <row r="56" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B56" s="1" t="s">
         <v>1</v>
       </c>
@@ -1259,8 +1259,8 @@
         <v>4</v>
       </c>
     </row>
-    <row r="57" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B57" s="5" t="s">
+    <row r="57" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="B57" s="11" t="s">
         <v>44</v>
       </c>
       <c r="C57" s="3" t="s">
@@ -1269,22 +1269,22 @@
       <c r="D57" s="3" t="s">
         <v>46</v>
       </c>
-      <c r="E57" s="15"/>
-    </row>
-    <row r="58" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B58" s="5"/>
+      <c r="E57" s="9"/>
+    </row>
+    <row r="58" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="B58" s="11"/>
       <c r="C58" s="3"/>
       <c r="D58" s="3"/>
-      <c r="E58" s="15"/>
-    </row>
-    <row r="59" spans="2:5" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B59" s="5"/>
+      <c r="E58" s="9"/>
+    </row>
+    <row r="59" spans="2:5" ht="30.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B59" s="11"/>
       <c r="C59" s="3"/>
       <c r="D59" s="3"/>
-      <c r="E59" s="15"/>
-    </row>
-    <row r="60" spans="2:5" ht="60" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B60" s="5" t="s">
+      <c r="E59" s="9"/>
+    </row>
+    <row r="60" spans="2:5" ht="60" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B60" s="11" t="s">
         <v>47</v>
       </c>
       <c r="C60" s="3" t="s">
@@ -1293,22 +1293,22 @@
       <c r="D60" s="3" t="s">
         <v>49</v>
       </c>
-      <c r="E60" s="15"/>
-    </row>
-    <row r="61" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B61" s="5"/>
+      <c r="E60" s="9"/>
+    </row>
+    <row r="61" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="B61" s="11"/>
       <c r="C61" s="3"/>
       <c r="D61" s="3"/>
-      <c r="E61" s="15"/>
-    </row>
-    <row r="62" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B62" s="5"/>
+      <c r="E61" s="9"/>
+    </row>
+    <row r="62" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="B62" s="11"/>
       <c r="C62" s="3"/>
       <c r="D62" s="3"/>
-      <c r="E62" s="15"/>
-    </row>
-    <row r="63" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B63" s="5" t="s">
+      <c r="E62" s="9"/>
+    </row>
+    <row r="63" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="B63" s="11" t="s">
         <v>50</v>
       </c>
       <c r="C63" s="3" t="s">
@@ -1317,68 +1317,68 @@
       <c r="D63" s="3" t="s">
         <v>52</v>
       </c>
-      <c r="E63" s="15"/>
-    </row>
-    <row r="64" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B64" s="5"/>
+      <c r="E63" s="9"/>
+    </row>
+    <row r="64" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="B64" s="11"/>
       <c r="C64" s="3"/>
       <c r="D64" s="3"/>
-      <c r="E64" s="15"/>
-    </row>
-    <row r="65" spans="2:5" ht="36" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B65" s="5"/>
+      <c r="E64" s="9"/>
+    </row>
+    <row r="65" spans="2:5" ht="36" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B65" s="11"/>
       <c r="C65" s="3"/>
       <c r="D65" s="3"/>
-      <c r="E65" s="15"/>
-    </row>
-    <row r="66" spans="2:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B66" s="2" t="s">
+      <c r="E65" s="9"/>
+    </row>
+    <row r="66" spans="2:5" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B66" s="4" t="s">
         <v>53</v>
       </c>
-      <c r="C66" s="16" t="s">
+      <c r="C66" s="10" t="s">
         <v>54</v>
       </c>
       <c r="D66" s="3" t="s">
         <v>55</v>
       </c>
-      <c r="E66" s="15"/>
-    </row>
-    <row r="67" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B67" s="2"/>
-      <c r="C67" s="16"/>
+      <c r="E66" s="9"/>
+    </row>
+    <row r="67" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="B67" s="4"/>
+      <c r="C67" s="10"/>
       <c r="D67" s="3"/>
-      <c r="E67" s="15"/>
-    </row>
-    <row r="68" spans="2:5" ht="48" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B68" s="2"/>
-      <c r="C68" s="16"/>
+      <c r="E67" s="9"/>
+    </row>
+    <row r="68" spans="2:5" ht="48" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B68" s="4"/>
+      <c r="C68" s="10"/>
       <c r="D68" s="3"/>
-      <c r="E68" s="15"/>
-    </row>
-    <row r="69" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B69" s="2"/>
+      <c r="E68" s="9"/>
+    </row>
+    <row r="69" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="B69" s="4"/>
       <c r="C69" s="3" t="s">
         <v>56</v>
       </c>
       <c r="D69" s="3" t="s">
         <v>57</v>
       </c>
-      <c r="E69" s="15"/>
-    </row>
-    <row r="70" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B70" s="2"/>
+      <c r="E69" s="9"/>
+    </row>
+    <row r="70" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="B70" s="4"/>
       <c r="C70" s="3"/>
       <c r="D70" s="3"/>
-      <c r="E70" s="15"/>
-    </row>
-    <row r="71" spans="2:5" ht="57.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B71" s="2"/>
+      <c r="E70" s="9"/>
+    </row>
+    <row r="71" spans="2:5" ht="57.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B71" s="4"/>
       <c r="C71" s="3"/>
       <c r="D71" s="3"/>
-      <c r="E71" s="15"/>
-    </row>
-    <row r="72" spans="2:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B72" s="2" t="s">
+      <c r="E71" s="9"/>
+    </row>
+    <row r="72" spans="2:5" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B72" s="4" t="s">
         <v>63</v>
       </c>
       <c r="C72" s="3" t="s">
@@ -1387,94 +1387,94 @@
       <c r="D72" s="3" t="s">
         <v>58</v>
       </c>
-      <c r="E72" s="15"/>
-    </row>
-    <row r="73" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B73" s="2"/>
+      <c r="E72" s="9"/>
+    </row>
+    <row r="73" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="B73" s="4"/>
       <c r="C73" s="3"/>
       <c r="D73" s="3"/>
-      <c r="E73" s="15"/>
-    </row>
-    <row r="74" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B74" s="2"/>
+      <c r="E73" s="9"/>
+    </row>
+    <row r="74" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="B74" s="4"/>
       <c r="C74" s="3"/>
       <c r="D74" s="3"/>
-      <c r="E74" s="15"/>
-    </row>
-    <row r="75" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B75" s="2"/>
+      <c r="E74" s="9"/>
+    </row>
+    <row r="75" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="B75" s="4"/>
       <c r="C75" s="3"/>
       <c r="D75" s="3"/>
-      <c r="E75" s="15"/>
-    </row>
-    <row r="76" spans="2:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B76" s="2"/>
+      <c r="E75" s="9"/>
+    </row>
+    <row r="76" spans="2:5" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B76" s="4"/>
       <c r="C76" s="3"/>
       <c r="D76" s="3"/>
-      <c r="E76" s="15"/>
-    </row>
-    <row r="77" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B77" s="2" t="s">
+      <c r="E76" s="9"/>
+    </row>
+    <row r="77" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="B77" s="4" t="s">
         <v>65</v>
       </c>
-      <c r="C77" s="16" t="s">
+      <c r="C77" s="10" t="s">
         <v>66</v>
       </c>
-      <c r="D77" s="16" t="s">
+      <c r="D77" s="10" t="s">
         <v>59</v>
       </c>
-      <c r="E77" s="15"/>
-    </row>
-    <row r="78" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B78" s="2"/>
-      <c r="C78" s="16"/>
-      <c r="D78" s="16"/>
-      <c r="E78" s="15"/>
-    </row>
-    <row r="79" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B79" s="2"/>
-      <c r="C79" s="16"/>
-      <c r="D79" s="16"/>
-      <c r="E79" s="15"/>
-    </row>
-    <row r="80" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B80" s="2"/>
-      <c r="C80" s="16"/>
-      <c r="D80" s="16"/>
-      <c r="E80" s="15"/>
-    </row>
-    <row r="81" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B81" s="5" t="s">
+      <c r="E77" s="9"/>
+    </row>
+    <row r="78" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="B78" s="4"/>
+      <c r="C78" s="10"/>
+      <c r="D78" s="10"/>
+      <c r="E78" s="9"/>
+    </row>
+    <row r="79" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="B79" s="4"/>
+      <c r="C79" s="10"/>
+      <c r="D79" s="10"/>
+      <c r="E79" s="9"/>
+    </row>
+    <row r="80" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="B80" s="4"/>
+      <c r="C80" s="10"/>
+      <c r="D80" s="10"/>
+      <c r="E80" s="9"/>
+    </row>
+    <row r="81" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="B81" s="11" t="s">
         <v>67</v>
       </c>
       <c r="C81" s="3" t="s">
         <v>68</v>
       </c>
-      <c r="D81" s="16" t="s">
+      <c r="D81" s="10" t="s">
         <v>60</v>
       </c>
-      <c r="E81" s="15"/>
-    </row>
-    <row r="82" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B82" s="5"/>
+      <c r="E81" s="9"/>
+    </row>
+    <row r="82" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="B82" s="11"/>
       <c r="C82" s="3"/>
-      <c r="D82" s="16"/>
-      <c r="E82" s="15"/>
-    </row>
-    <row r="83" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B83" s="5"/>
+      <c r="D82" s="10"/>
+      <c r="E82" s="9"/>
+    </row>
+    <row r="83" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="B83" s="11"/>
       <c r="C83" s="3"/>
-      <c r="D83" s="16"/>
-      <c r="E83" s="15"/>
-    </row>
-    <row r="84" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B84" s="5"/>
+      <c r="D83" s="10"/>
+      <c r="E83" s="9"/>
+    </row>
+    <row r="84" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="B84" s="11"/>
       <c r="C84" s="3"/>
-      <c r="D84" s="16"/>
-      <c r="E84" s="15"/>
-    </row>
-    <row r="85" spans="2:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B85" s="2" t="s">
+      <c r="D84" s="10"/>
+      <c r="E84" s="9"/>
+    </row>
+    <row r="85" spans="2:5" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B85" s="4" t="s">
         <v>69</v>
       </c>
       <c r="C85" s="3" t="s">
@@ -1483,34 +1483,34 @@
       <c r="D85" s="3" t="s">
         <v>61</v>
       </c>
-      <c r="E85" s="15"/>
-    </row>
-    <row r="86" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B86" s="2"/>
+      <c r="E85" s="9"/>
+    </row>
+    <row r="86" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="B86" s="4"/>
       <c r="C86" s="3"/>
       <c r="D86" s="3"/>
-      <c r="E86" s="15"/>
-    </row>
-    <row r="87" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B87" s="2"/>
+      <c r="E86" s="9"/>
+    </row>
+    <row r="87" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="B87" s="4"/>
       <c r="C87" s="3"/>
       <c r="D87" s="3"/>
-      <c r="E87" s="15"/>
-    </row>
-    <row r="88" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B88" s="2"/>
+      <c r="E87" s="9"/>
+    </row>
+    <row r="88" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="B88" s="4"/>
       <c r="C88" s="3"/>
       <c r="D88" s="3"/>
-      <c r="E88" s="15"/>
-    </row>
-    <row r="89" spans="2:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B89" s="2"/>
+      <c r="E88" s="9"/>
+    </row>
+    <row r="89" spans="2:5" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B89" s="4"/>
       <c r="C89" s="3"/>
       <c r="D89" s="3"/>
-      <c r="E89" s="15"/>
-    </row>
-    <row r="90" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B90" s="2" t="s">
+      <c r="E89" s="9"/>
+    </row>
+    <row r="90" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="B90" s="4" t="s">
         <v>71</v>
       </c>
       <c r="C90" s="3" t="s">
@@ -1519,41 +1519,41 @@
       <c r="D90" s="3" t="s">
         <v>62</v>
       </c>
-      <c r="E90" s="15"/>
-    </row>
-    <row r="91" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B91" s="2"/>
+      <c r="E90" s="9"/>
+    </row>
+    <row r="91" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="B91" s="4"/>
       <c r="C91" s="3"/>
       <c r="D91" s="3"/>
-      <c r="E91" s="15"/>
-    </row>
-    <row r="92" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B92" s="2"/>
+      <c r="E91" s="9"/>
+    </row>
+    <row r="92" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="B92" s="4"/>
       <c r="C92" s="3"/>
       <c r="D92" s="3"/>
-      <c r="E92" s="15"/>
-    </row>
-    <row r="93" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B93" s="2"/>
+      <c r="E92" s="9"/>
+    </row>
+    <row r="93" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="B93" s="4"/>
       <c r="C93" s="3"/>
       <c r="D93" s="3"/>
-      <c r="E93" s="15"/>
-    </row>
-    <row r="94" spans="2:5" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B94" s="2"/>
+      <c r="E93" s="9"/>
+    </row>
+    <row r="94" spans="2:5" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B94" s="4"/>
       <c r="C94" s="3"/>
       <c r="D94" s="3"/>
-      <c r="E94" s="15"/>
-    </row>
-    <row r="96" spans="2:5" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="B96" s="4" t="s">
+      <c r="E94" s="9"/>
+    </row>
+    <row r="96" spans="2:5" ht="18.5" x14ac:dyDescent="0.45">
+      <c r="B96" s="2" t="s">
         <v>73</v>
       </c>
-      <c r="C96" s="4"/>
-      <c r="D96" s="4"/>
-      <c r="E96" s="4"/>
-    </row>
-    <row r="97" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="C96" s="2"/>
+      <c r="D96" s="2"/>
+      <c r="E96" s="2"/>
+    </row>
+    <row r="97" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B97" s="1" t="s">
         <v>1</v>
       </c>
@@ -1567,8 +1567,8 @@
         <v>4</v>
       </c>
     </row>
-    <row r="98" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B98" s="2" t="s">
+    <row r="98" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="B98" s="4" t="s">
         <v>74</v>
       </c>
       <c r="C98" s="3" t="s">
@@ -1577,28 +1577,28 @@
       <c r="D98" s="3" t="s">
         <v>76</v>
       </c>
-      <c r="E98" s="9"/>
-    </row>
-    <row r="99" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B99" s="2"/>
+      <c r="E98" s="5"/>
+    </row>
+    <row r="99" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="B99" s="4"/>
       <c r="C99" s="3"/>
       <c r="D99" s="3"/>
-      <c r="E99" s="10"/>
-    </row>
-    <row r="100" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B100" s="2"/>
+      <c r="E99" s="6"/>
+    </row>
+    <row r="100" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="B100" s="4"/>
       <c r="C100" s="3"/>
       <c r="D100" s="3"/>
-      <c r="E100" s="10"/>
-    </row>
-    <row r="101" spans="2:5" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B101" s="2"/>
+      <c r="E100" s="6"/>
+    </row>
+    <row r="101" spans="2:5" ht="32.25" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B101" s="4"/>
       <c r="C101" s="3"/>
       <c r="D101" s="3"/>
-      <c r="E101" s="11"/>
-    </row>
-    <row r="102" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B102" s="2" t="s">
+      <c r="E101" s="7"/>
+    </row>
+    <row r="102" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="B102" s="4" t="s">
         <v>77</v>
       </c>
       <c r="C102" s="3" t="s">
@@ -1607,28 +1607,28 @@
       <c r="D102" s="3" t="s">
         <v>79</v>
       </c>
-      <c r="E102" s="9"/>
-    </row>
-    <row r="103" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B103" s="2"/>
+      <c r="E102" s="5"/>
+    </row>
+    <row r="103" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="B103" s="4"/>
       <c r="C103" s="3"/>
       <c r="D103" s="3"/>
-      <c r="E103" s="10"/>
-    </row>
-    <row r="104" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B104" s="2"/>
+      <c r="E103" s="6"/>
+    </row>
+    <row r="104" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="B104" s="4"/>
       <c r="C104" s="3"/>
       <c r="D104" s="3"/>
-      <c r="E104" s="10"/>
-    </row>
-    <row r="105" spans="2:5" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B105" s="2"/>
+      <c r="E104" s="6"/>
+    </row>
+    <row r="105" spans="2:5" ht="32.25" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B105" s="4"/>
       <c r="C105" s="3"/>
       <c r="D105" s="3"/>
-      <c r="E105" s="11"/>
-    </row>
-    <row r="106" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B106" s="2" t="s">
+      <c r="E105" s="7"/>
+    </row>
+    <row r="106" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="B106" s="4" t="s">
         <v>80</v>
       </c>
       <c r="C106" s="3" t="s">
@@ -1637,35 +1637,35 @@
       <c r="D106" s="3" t="s">
         <v>82</v>
       </c>
-      <c r="E106" s="9"/>
-    </row>
-    <row r="107" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B107" s="2"/>
+      <c r="E106" s="5"/>
+    </row>
+    <row r="107" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="B107" s="4"/>
       <c r="C107" s="3"/>
       <c r="D107" s="3"/>
-      <c r="E107" s="10"/>
-    </row>
-    <row r="108" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B108" s="2"/>
+      <c r="E107" s="6"/>
+    </row>
+    <row r="108" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="B108" s="4"/>
       <c r="C108" s="3"/>
       <c r="D108" s="3"/>
-      <c r="E108" s="10"/>
-    </row>
-    <row r="109" spans="2:5" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B109" s="2"/>
+      <c r="E108" s="6"/>
+    </row>
+    <row r="109" spans="2:5" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B109" s="4"/>
       <c r="C109" s="3"/>
       <c r="D109" s="3"/>
-      <c r="E109" s="11"/>
-    </row>
-    <row r="112" spans="2:5" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="B112" s="4" t="s">
+      <c r="E109" s="7"/>
+    </row>
+    <row r="112" spans="2:5" ht="18.5" x14ac:dyDescent="0.45">
+      <c r="B112" s="2" t="s">
         <v>83</v>
       </c>
-      <c r="C112" s="4"/>
-      <c r="D112" s="4"/>
-      <c r="E112" s="4"/>
-    </row>
-    <row r="113" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="C112" s="2"/>
+      <c r="D112" s="2"/>
+      <c r="E112" s="2"/>
+    </row>
+    <row r="113" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B113" s="1" t="s">
         <v>1</v>
       </c>
@@ -1679,8 +1679,8 @@
         <v>4</v>
       </c>
     </row>
-    <row r="114" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B114" s="2" t="s">
+    <row r="114" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="B114" s="4" t="s">
         <v>84</v>
       </c>
       <c r="C114" s="3" t="s">
@@ -1689,28 +1689,28 @@
       <c r="D114" s="3" t="s">
         <v>86</v>
       </c>
-      <c r="E114" s="9"/>
-    </row>
-    <row r="115" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B115" s="2"/>
+      <c r="E114" s="5"/>
+    </row>
+    <row r="115" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="B115" s="4"/>
       <c r="C115" s="3"/>
       <c r="D115" s="3"/>
-      <c r="E115" s="10"/>
-    </row>
-    <row r="116" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B116" s="2"/>
+      <c r="E115" s="6"/>
+    </row>
+    <row r="116" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="B116" s="4"/>
       <c r="C116" s="3"/>
       <c r="D116" s="3"/>
-      <c r="E116" s="10"/>
-    </row>
-    <row r="117" spans="2:5" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B117" s="2"/>
+      <c r="E116" s="6"/>
+    </row>
+    <row r="117" spans="2:5" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B117" s="4"/>
       <c r="C117" s="3"/>
       <c r="D117" s="3"/>
-      <c r="E117" s="11"/>
-    </row>
-    <row r="118" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B118" s="2" t="s">
+      <c r="E117" s="7"/>
+    </row>
+    <row r="118" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="B118" s="4" t="s">
         <v>87</v>
       </c>
       <c r="C118" s="3" t="s">
@@ -1719,35 +1719,35 @@
       <c r="D118" s="3" t="s">
         <v>88</v>
       </c>
-      <c r="E118" s="9"/>
-    </row>
-    <row r="119" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B119" s="2"/>
+      <c r="E118" s="5"/>
+    </row>
+    <row r="119" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="B119" s="4"/>
       <c r="C119" s="3"/>
       <c r="D119" s="3"/>
-      <c r="E119" s="10"/>
-    </row>
-    <row r="120" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B120" s="2"/>
+      <c r="E119" s="6"/>
+    </row>
+    <row r="120" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="B120" s="4"/>
       <c r="C120" s="3"/>
       <c r="D120" s="3"/>
-      <c r="E120" s="10"/>
-    </row>
-    <row r="121" spans="2:5" ht="47.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B121" s="2"/>
+      <c r="E120" s="6"/>
+    </row>
+    <row r="121" spans="2:5" ht="47.25" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B121" s="4"/>
       <c r="C121" s="3"/>
       <c r="D121" s="3"/>
-      <c r="E121" s="11"/>
-    </row>
-    <row r="123" spans="2:5" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="B123" s="4" t="s">
+      <c r="E121" s="7"/>
+    </row>
+    <row r="123" spans="2:5" ht="18.5" x14ac:dyDescent="0.45">
+      <c r="B123" s="2" t="s">
         <v>89</v>
       </c>
-      <c r="C123" s="4"/>
-      <c r="D123" s="4"/>
-      <c r="E123" s="4"/>
-    </row>
-    <row r="124" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="C123" s="2"/>
+      <c r="D123" s="2"/>
+      <c r="E123" s="2"/>
+    </row>
+    <row r="124" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B124" s="1" t="s">
         <v>1</v>
       </c>
@@ -1761,8 +1761,8 @@
         <v>4</v>
       </c>
     </row>
-    <row r="125" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B125" s="2" t="s">
+    <row r="125" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="B125" s="4" t="s">
         <v>90</v>
       </c>
       <c r="C125" s="3" t="s">
@@ -1771,58 +1771,58 @@
       <c r="D125" s="3" t="s">
         <v>92</v>
       </c>
-      <c r="E125" s="9"/>
-    </row>
-    <row r="126" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B126" s="2"/>
+      <c r="E125" s="5"/>
+    </row>
+    <row r="126" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="B126" s="4"/>
       <c r="C126" s="3"/>
       <c r="D126" s="3"/>
-      <c r="E126" s="10"/>
-    </row>
-    <row r="127" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B127" s="2"/>
+      <c r="E126" s="6"/>
+    </row>
+    <row r="127" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="B127" s="4"/>
       <c r="C127" s="3"/>
       <c r="D127" s="3"/>
-      <c r="E127" s="10"/>
-    </row>
-    <row r="128" spans="2:5" ht="44.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B128" s="2"/>
+      <c r="E127" s="6"/>
+    </row>
+    <row r="128" spans="2:5" ht="44.25" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B128" s="4"/>
       <c r="C128" s="3"/>
       <c r="D128" s="3"/>
-      <c r="E128" s="11"/>
-    </row>
-    <row r="129" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B129" s="2" t="s">
+      <c r="E128" s="7"/>
+    </row>
+    <row r="129" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="B129" s="4" t="s">
         <v>93</v>
       </c>
-      <c r="C129" s="17" t="s">
+      <c r="C129" s="8" t="s">
         <v>94</v>
       </c>
       <c r="D129" s="3" t="s">
         <v>95</v>
       </c>
-      <c r="E129" s="9"/>
-    </row>
-    <row r="130" spans="2:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B130" s="2"/>
-      <c r="C130" s="17"/>
+      <c r="E129" s="5"/>
+    </row>
+    <row r="130" spans="2:5" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B130" s="4"/>
+      <c r="C130" s="8"/>
       <c r="D130" s="3"/>
-      <c r="E130" s="10"/>
-    </row>
-    <row r="131" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B131" s="2"/>
-      <c r="C131" s="17"/>
+      <c r="E130" s="6"/>
+    </row>
+    <row r="131" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="B131" s="4"/>
+      <c r="C131" s="8"/>
       <c r="D131" s="3"/>
-      <c r="E131" s="10"/>
-    </row>
-    <row r="132" spans="2:5" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B132" s="2"/>
-      <c r="C132" s="17"/>
+      <c r="E131" s="6"/>
+    </row>
+    <row r="132" spans="2:5" ht="45" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B132" s="4"/>
+      <c r="C132" s="8"/>
       <c r="D132" s="3"/>
-      <c r="E132" s="11"/>
-    </row>
-    <row r="133" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B133" s="2" t="s">
+      <c r="E132" s="7"/>
+    </row>
+    <row r="133" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="B133" s="4" t="s">
         <v>97</v>
       </c>
       <c r="C133" s="3" t="s">
@@ -1831,47 +1831,47 @@
       <c r="D133" s="3" t="s">
         <v>99</v>
       </c>
-      <c r="E133" s="9"/>
-    </row>
-    <row r="134" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B134" s="2"/>
+      <c r="E133" s="5"/>
+    </row>
+    <row r="134" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="B134" s="4"/>
       <c r="C134" s="3"/>
       <c r="D134" s="3"/>
-      <c r="E134" s="10"/>
-    </row>
-    <row r="135" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B135" s="2"/>
+      <c r="E134" s="6"/>
+    </row>
+    <row r="135" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="B135" s="4"/>
       <c r="C135" s="3"/>
       <c r="D135" s="3"/>
-      <c r="E135" s="10"/>
-    </row>
-    <row r="136" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B136" s="2"/>
+      <c r="E135" s="6"/>
+    </row>
+    <row r="136" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="B136" s="4"/>
       <c r="C136" s="3"/>
       <c r="D136" s="3"/>
-      <c r="E136" s="10"/>
-    </row>
-    <row r="137" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B137" s="2"/>
+      <c r="E136" s="6"/>
+    </row>
+    <row r="137" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="B137" s="4"/>
       <c r="C137" s="3"/>
       <c r="D137" s="3"/>
-      <c r="E137" s="10"/>
-    </row>
-    <row r="138" spans="2:5" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B138" s="2"/>
+      <c r="E137" s="6"/>
+    </row>
+    <row r="138" spans="2:5" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B138" s="4"/>
       <c r="C138" s="3"/>
       <c r="D138" s="3"/>
-      <c r="E138" s="11"/>
-    </row>
-    <row r="140" spans="2:5" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="B140" s="4" t="s">
+      <c r="E138" s="7"/>
+    </row>
+    <row r="140" spans="2:5" ht="18.5" x14ac:dyDescent="0.45">
+      <c r="B140" s="2" t="s">
         <v>100</v>
       </c>
-      <c r="C140" s="4"/>
-      <c r="D140" s="4"/>
-      <c r="E140" s="4"/>
-    </row>
-    <row r="141" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="C140" s="2"/>
+      <c r="D140" s="2"/>
+      <c r="E140" s="2"/>
+    </row>
+    <row r="141" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B141" s="1" t="s">
         <v>1</v>
       </c>
@@ -1885,8 +1885,8 @@
         <v>4</v>
       </c>
     </row>
-    <row r="142" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B142" s="2" t="s">
+    <row r="142" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="B142" s="4" t="s">
         <v>101</v>
       </c>
       <c r="C142" s="3" t="s">
@@ -1895,27 +1895,27 @@
       <c r="D142" s="3" t="s">
         <v>103</v>
       </c>
-      <c r="E142" s="9"/>
-    </row>
-    <row r="143" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B143" s="2"/>
+      <c r="E142" s="5"/>
+    </row>
+    <row r="143" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="B143" s="4"/>
       <c r="C143" s="3"/>
       <c r="D143" s="3"/>
-      <c r="E143" s="10"/>
-    </row>
-    <row r="144" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B144" s="2"/>
+      <c r="E143" s="6"/>
+    </row>
+    <row r="144" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="B144" s="4"/>
       <c r="C144" s="3"/>
       <c r="D144" s="3"/>
-      <c r="E144" s="10"/>
-    </row>
-    <row r="145" spans="2:5" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B145" s="2"/>
+      <c r="E144" s="6"/>
+    </row>
+    <row r="145" spans="2:5" ht="29.25" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B145" s="4"/>
       <c r="C145" s="3"/>
       <c r="D145" s="3"/>
-      <c r="E145" s="11"/>
-    </row>
-    <row r="146" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="E145" s="7"/>
+    </row>
+    <row r="146" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B146" s="3" t="s">
         <v>104</v>
       </c>
@@ -1925,139 +1925,61 @@
       <c r="D146" s="3" t="s">
         <v>106</v>
       </c>
-      <c r="E146" s="9"/>
-    </row>
-    <row r="147" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="E146" s="5"/>
+    </row>
+    <row r="147" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B147" s="3"/>
       <c r="C147" s="3"/>
       <c r="D147" s="3"/>
-      <c r="E147" s="10"/>
-    </row>
-    <row r="148" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="E147" s="6"/>
+    </row>
+    <row r="148" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B148" s="3"/>
       <c r="C148" s="3"/>
       <c r="D148" s="3"/>
-      <c r="E148" s="10"/>
-    </row>
-    <row r="149" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="E148" s="6"/>
+    </row>
+    <row r="149" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B149" s="3"/>
       <c r="C149" s="3"/>
       <c r="D149" s="3"/>
-      <c r="E149" s="10"/>
-    </row>
-    <row r="150" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="E149" s="6"/>
+    </row>
+    <row r="150" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B150" s="3"/>
       <c r="C150" s="3"/>
       <c r="D150" s="3"/>
-      <c r="E150" s="10"/>
-    </row>
-    <row r="151" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="E150" s="6"/>
+    </row>
+    <row r="151" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B151" s="3"/>
       <c r="C151" s="3"/>
       <c r="D151" s="3"/>
-      <c r="E151" s="10"/>
-    </row>
-    <row r="152" spans="2:5" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E151" s="6"/>
+    </row>
+    <row r="152" spans="2:5" ht="33.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B152" s="3"/>
       <c r="C152" s="3"/>
       <c r="D152" s="3"/>
-      <c r="E152" s="11"/>
+      <c r="E152" s="7"/>
     </row>
   </sheetData>
   <mergeCells count="132">
-    <mergeCell ref="B140:E140"/>
-    <mergeCell ref="C142:C145"/>
-    <mergeCell ref="D142:D145"/>
-    <mergeCell ref="B142:B145"/>
-    <mergeCell ref="D146:D152"/>
-    <mergeCell ref="C146:C152"/>
-    <mergeCell ref="B146:B152"/>
-    <mergeCell ref="E142:E145"/>
-    <mergeCell ref="E146:E152"/>
-    <mergeCell ref="B123:E123"/>
-    <mergeCell ref="C125:C128"/>
-    <mergeCell ref="D125:D128"/>
-    <mergeCell ref="B125:B128"/>
-    <mergeCell ref="C129:C132"/>
-    <mergeCell ref="D129:D132"/>
-    <mergeCell ref="B129:B132"/>
-    <mergeCell ref="D133:D138"/>
-    <mergeCell ref="C133:C138"/>
-    <mergeCell ref="B133:B138"/>
-    <mergeCell ref="E125:E128"/>
-    <mergeCell ref="E129:E132"/>
-    <mergeCell ref="E133:E138"/>
-    <mergeCell ref="B112:E112"/>
-    <mergeCell ref="C114:C117"/>
-    <mergeCell ref="D114:D117"/>
-    <mergeCell ref="B114:B117"/>
-    <mergeCell ref="C118:C121"/>
-    <mergeCell ref="D118:D121"/>
-    <mergeCell ref="B118:B121"/>
-    <mergeCell ref="E114:E117"/>
-    <mergeCell ref="E118:E121"/>
-    <mergeCell ref="C106:C109"/>
-    <mergeCell ref="D106:D109"/>
-    <mergeCell ref="B106:B109"/>
-    <mergeCell ref="E98:E101"/>
-    <mergeCell ref="E102:E105"/>
-    <mergeCell ref="E106:E109"/>
-    <mergeCell ref="B96:E96"/>
-    <mergeCell ref="C98:C101"/>
-    <mergeCell ref="D98:D101"/>
-    <mergeCell ref="B98:B101"/>
-    <mergeCell ref="C102:C105"/>
-    <mergeCell ref="D102:D105"/>
-    <mergeCell ref="B102:B105"/>
-    <mergeCell ref="C90:C94"/>
-    <mergeCell ref="D90:D94"/>
-    <mergeCell ref="B90:B94"/>
-    <mergeCell ref="E72:E76"/>
-    <mergeCell ref="E77:E80"/>
-    <mergeCell ref="E81:E84"/>
-    <mergeCell ref="E85:E89"/>
-    <mergeCell ref="E90:E94"/>
-    <mergeCell ref="D81:D84"/>
-    <mergeCell ref="C81:C84"/>
-    <mergeCell ref="B81:B84"/>
-    <mergeCell ref="D85:D89"/>
-    <mergeCell ref="C85:C89"/>
-    <mergeCell ref="B85:B89"/>
-    <mergeCell ref="D72:D76"/>
-    <mergeCell ref="B66:B71"/>
-    <mergeCell ref="C72:C76"/>
-    <mergeCell ref="B72:B76"/>
-    <mergeCell ref="C77:C80"/>
-    <mergeCell ref="D77:D80"/>
-    <mergeCell ref="B77:B80"/>
-    <mergeCell ref="E66:E68"/>
-    <mergeCell ref="E69:E71"/>
-    <mergeCell ref="C66:C68"/>
-    <mergeCell ref="D66:D68"/>
-    <mergeCell ref="C69:C71"/>
-    <mergeCell ref="D69:D71"/>
-    <mergeCell ref="C63:C65"/>
-    <mergeCell ref="D63:D65"/>
-    <mergeCell ref="B63:B65"/>
-    <mergeCell ref="E57:E59"/>
-    <mergeCell ref="E60:E62"/>
-    <mergeCell ref="E63:E65"/>
-    <mergeCell ref="B39:E39"/>
-    <mergeCell ref="C41:C43"/>
-    <mergeCell ref="C44:C46"/>
-    <mergeCell ref="C47:C49"/>
-    <mergeCell ref="C60:C62"/>
-    <mergeCell ref="D60:D62"/>
-    <mergeCell ref="B60:B62"/>
-    <mergeCell ref="B55:E55"/>
-    <mergeCell ref="C57:C59"/>
-    <mergeCell ref="D57:D59"/>
-    <mergeCell ref="B57:B59"/>
-    <mergeCell ref="E47:E49"/>
-    <mergeCell ref="C50:C52"/>
-    <mergeCell ref="D50:D52"/>
-    <mergeCell ref="B50:B52"/>
-    <mergeCell ref="E50:E52"/>
+    <mergeCell ref="B2:E2"/>
+    <mergeCell ref="C4:C6"/>
+    <mergeCell ref="C7:C9"/>
+    <mergeCell ref="B4:B9"/>
+    <mergeCell ref="D19:D22"/>
+    <mergeCell ref="B19:B25"/>
+    <mergeCell ref="D30:D33"/>
+    <mergeCell ref="D34:D36"/>
+    <mergeCell ref="D23:D25"/>
+    <mergeCell ref="C10:C12"/>
+    <mergeCell ref="C13:C15"/>
+    <mergeCell ref="C16:C18"/>
+    <mergeCell ref="C23:C25"/>
+    <mergeCell ref="B10:B18"/>
+    <mergeCell ref="C19:C22"/>
     <mergeCell ref="G2:H2"/>
     <mergeCell ref="G3:H3"/>
     <mergeCell ref="G4:H4"/>
@@ -2082,21 +2004,99 @@
     <mergeCell ref="E10:E18"/>
     <mergeCell ref="E19:E25"/>
     <mergeCell ref="E26:E36"/>
-    <mergeCell ref="D30:D33"/>
-    <mergeCell ref="D34:D36"/>
-    <mergeCell ref="D23:D25"/>
-    <mergeCell ref="C10:C12"/>
-    <mergeCell ref="C13:C15"/>
-    <mergeCell ref="C16:C18"/>
-    <mergeCell ref="C23:C25"/>
-    <mergeCell ref="B10:B18"/>
-    <mergeCell ref="C19:C22"/>
-    <mergeCell ref="B2:E2"/>
-    <mergeCell ref="C4:C6"/>
-    <mergeCell ref="C7:C9"/>
-    <mergeCell ref="B4:B9"/>
-    <mergeCell ref="D19:D22"/>
-    <mergeCell ref="B19:B25"/>
+    <mergeCell ref="C63:C65"/>
+    <mergeCell ref="D63:D65"/>
+    <mergeCell ref="B63:B65"/>
+    <mergeCell ref="E57:E59"/>
+    <mergeCell ref="E60:E62"/>
+    <mergeCell ref="E63:E65"/>
+    <mergeCell ref="B39:E39"/>
+    <mergeCell ref="C41:C43"/>
+    <mergeCell ref="C44:C46"/>
+    <mergeCell ref="C47:C49"/>
+    <mergeCell ref="C60:C62"/>
+    <mergeCell ref="D60:D62"/>
+    <mergeCell ref="B60:B62"/>
+    <mergeCell ref="B55:E55"/>
+    <mergeCell ref="C57:C59"/>
+    <mergeCell ref="D57:D59"/>
+    <mergeCell ref="B57:B59"/>
+    <mergeCell ref="E47:E49"/>
+    <mergeCell ref="C50:C52"/>
+    <mergeCell ref="D50:D52"/>
+    <mergeCell ref="B50:B52"/>
+    <mergeCell ref="E50:E52"/>
+    <mergeCell ref="B66:B71"/>
+    <mergeCell ref="C72:C76"/>
+    <mergeCell ref="B72:B76"/>
+    <mergeCell ref="C77:C80"/>
+    <mergeCell ref="D77:D80"/>
+    <mergeCell ref="B77:B80"/>
+    <mergeCell ref="E66:E68"/>
+    <mergeCell ref="E69:E71"/>
+    <mergeCell ref="C66:C68"/>
+    <mergeCell ref="D66:D68"/>
+    <mergeCell ref="C69:C71"/>
+    <mergeCell ref="D69:D71"/>
+    <mergeCell ref="C90:C94"/>
+    <mergeCell ref="D90:D94"/>
+    <mergeCell ref="B90:B94"/>
+    <mergeCell ref="E72:E76"/>
+    <mergeCell ref="E77:E80"/>
+    <mergeCell ref="E81:E84"/>
+    <mergeCell ref="E85:E89"/>
+    <mergeCell ref="E90:E94"/>
+    <mergeCell ref="D81:D84"/>
+    <mergeCell ref="C81:C84"/>
+    <mergeCell ref="B81:B84"/>
+    <mergeCell ref="D85:D89"/>
+    <mergeCell ref="C85:C89"/>
+    <mergeCell ref="B85:B89"/>
+    <mergeCell ref="D72:D76"/>
+    <mergeCell ref="C106:C109"/>
+    <mergeCell ref="D106:D109"/>
+    <mergeCell ref="B106:B109"/>
+    <mergeCell ref="E98:E101"/>
+    <mergeCell ref="E102:E105"/>
+    <mergeCell ref="E106:E109"/>
+    <mergeCell ref="B96:E96"/>
+    <mergeCell ref="C98:C101"/>
+    <mergeCell ref="D98:D101"/>
+    <mergeCell ref="B98:B101"/>
+    <mergeCell ref="C102:C105"/>
+    <mergeCell ref="D102:D105"/>
+    <mergeCell ref="B102:B105"/>
+    <mergeCell ref="B112:E112"/>
+    <mergeCell ref="C114:C117"/>
+    <mergeCell ref="D114:D117"/>
+    <mergeCell ref="B114:B117"/>
+    <mergeCell ref="C118:C121"/>
+    <mergeCell ref="D118:D121"/>
+    <mergeCell ref="B118:B121"/>
+    <mergeCell ref="E114:E117"/>
+    <mergeCell ref="E118:E121"/>
+    <mergeCell ref="B123:E123"/>
+    <mergeCell ref="C125:C128"/>
+    <mergeCell ref="D125:D128"/>
+    <mergeCell ref="B125:B128"/>
+    <mergeCell ref="C129:C132"/>
+    <mergeCell ref="D129:D132"/>
+    <mergeCell ref="B129:B132"/>
+    <mergeCell ref="D133:D138"/>
+    <mergeCell ref="C133:C138"/>
+    <mergeCell ref="B133:B138"/>
+    <mergeCell ref="E125:E128"/>
+    <mergeCell ref="E129:E132"/>
+    <mergeCell ref="E133:E138"/>
+    <mergeCell ref="B140:E140"/>
+    <mergeCell ref="C142:C145"/>
+    <mergeCell ref="D142:D145"/>
+    <mergeCell ref="B142:B145"/>
+    <mergeCell ref="D146:D152"/>
+    <mergeCell ref="C146:C152"/>
+    <mergeCell ref="B146:B152"/>
+    <mergeCell ref="E142:E145"/>
+    <mergeCell ref="E146:E152"/>
   </mergeCells>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>